<commit_message>
[doc]: updated asvs doc
</commit_message>
<xml_diff>
--- a/deliverable/v4-ASVS-checklist-en.xlsx
+++ b/deliverable/v4-ASVS-checklist-en.xlsx
@@ -3482,7 +3482,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3692,13 +3692,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="44014047"/>
-        <c:axId val="79675496"/>
+        <c:axId val="96512831"/>
+        <c:axId val="78617493"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="44014047"/>
+        <c:axId val="96512831"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3735,7 +3735,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79675496"/>
+        <c:crossAx val="78617493"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3743,7 +3743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79675496"/>
+        <c:axId val="78617493"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3785,7 +3785,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44014047"/>
+        <c:crossAx val="96512831"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3850,9 +3850,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1718640</xdr:colOff>
+      <xdr:colOff>1718280</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3861,7 +3861,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="4510800"/>
-        <a:ext cx="11146320" cy="9333360"/>
+        <a:ext cx="11146680" cy="9333000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6329,8 +6329,8 @@
   </sheetPr>
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>